<commit_message>
refactor: adjusted flow to getting buys of the user
</commit_message>
<xml_diff>
--- a/testexcel.xlsx
+++ b/testexcel.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="201">
   <si>
     <t>NOME CLIENTE</t>
   </si>
@@ -230,6 +230,24 @@
     <t>60770a98-8346-474a-9115-7752ba6a7685</t>
   </si>
   <si>
+    <t>Eduardo Santos</t>
+  </si>
+  <si>
+    <t>21/11/2024 12:08:40</t>
+  </si>
+  <si>
+    <t>8a14281a-8803-423f-8347-f606cf47362a</t>
+  </si>
+  <si>
+    <t>Relógio</t>
+  </si>
+  <si>
+    <t>05/12/2024 22:44:37</t>
+  </si>
+  <si>
+    <t>c9ed941a-85a3-4024-880d-1b56d2821cb2</t>
+  </si>
+  <si>
     <t>Felipe Silva</t>
   </si>
   <si>
@@ -266,6 +284,63 @@
     <t>13efa55c-baf4-4095-b451-2971c480bcbf</t>
   </si>
   <si>
+    <t>João Pedro</t>
+  </si>
+  <si>
+    <t>21/11/2024 12:08:47</t>
+  </si>
+  <si>
+    <t>fdcf1c11-1cee-4aac-9e25-c670bd268b4e</t>
+  </si>
+  <si>
+    <t>Carregador</t>
+  </si>
+  <si>
+    <t>07/12/2024 15:10:38</t>
+  </si>
+  <si>
+    <t>Caderno</t>
+  </si>
+  <si>
+    <t>07/12/2024 15:11:40</t>
+  </si>
+  <si>
+    <t>0999422a-9c6d-4de6-b026-018452584fa3</t>
+  </si>
+  <si>
+    <t>Mariana Duarte</t>
+  </si>
+  <si>
+    <t>21/11/2024 12:08:51</t>
+  </si>
+  <si>
+    <t>c2cada87-cbd6-4723-879a-bf4d4a4a692b</t>
+  </si>
+  <si>
+    <t>05/12/2024 20:29:21</t>
+  </si>
+  <si>
+    <t>05/12/2024 20:30:41</t>
+  </si>
+  <si>
+    <t>dbe7e5a5-f3a9-433e-b6a1-7761ac6e304e</t>
+  </si>
+  <si>
+    <t>Rafael Barbosa</t>
+  </si>
+  <si>
+    <t>21/11/2024 12:08:57</t>
+  </si>
+  <si>
+    <t>140c0fc3-d50c-4272-91fd-5523b7d4d5d9</t>
+  </si>
+  <si>
+    <t>05/12/2024 22:45:35</t>
+  </si>
+  <si>
+    <t>b6338573-da9c-4637-9119-639a77e1d76a</t>
+  </si>
+  <si>
     <t xml:space="preserve">Cicero </t>
   </si>
   <si>
@@ -293,9 +368,6 @@
     <t>efb9658e-8387-4d5f-a2b8-68fd3347ef9c</t>
   </si>
   <si>
-    <t>Caderno</t>
-  </si>
-  <si>
     <t>23/11/2024 00:21:38</t>
   </si>
   <si>
@@ -392,9 +464,6 @@
     <t>0f736aed-7f3f-4e63-94e0-75c5956d773c</t>
   </si>
   <si>
-    <t>Relógio</t>
-  </si>
-  <si>
     <t>228cf1cb-ef25-46e3-9267-56525800db2c</t>
   </si>
   <si>
@@ -452,6 +521,12 @@
     <t>8236ba84-e165-4dbe-967a-b82ba25dd90d</t>
   </si>
   <si>
+    <t>Pen Drive</t>
+  </si>
+  <si>
+    <t>05/12/2024 20:27:51</t>
+  </si>
+  <si>
     <t>03/12/2024 19:39:59</t>
   </si>
   <si>
@@ -492,6 +567,54 @@
   </si>
   <si>
     <t>b2b213b4-dffa-4736-9c21-2f694ab495a7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Guilherme Alves </t>
+  </si>
+  <si>
+    <t>05/12/2024 20:34:00</t>
+  </si>
+  <si>
+    <t>76c9605b-0901-4763-9123-7c945510001d</t>
+  </si>
+  <si>
+    <t>05/12/2024 22:37:02</t>
+  </si>
+  <si>
+    <t>07/12/2024 15:45:43</t>
+  </si>
+  <si>
+    <t>12f96c1b-0c88-46fe-b4a0-636c9d68b68f</t>
+  </si>
+  <si>
+    <t>07/12/2024 15:46:04</t>
+  </si>
+  <si>
+    <t>678b009b-d277-41d5-9d9f-ae6581810410</t>
+  </si>
+  <si>
+    <t>Ysis</t>
+  </si>
+  <si>
+    <t>05/12/2024 22:36:27</t>
+  </si>
+  <si>
+    <t>cdd8348c-1cf2-4c0e-9d9d-1f44d9804175</t>
+  </si>
+  <si>
+    <t>c8224efd-2c33-45d0-af6f-b05a447727f6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ysis </t>
+  </si>
+  <si>
+    <t>05/12/2024 22:38:42</t>
+  </si>
+  <si>
+    <t>d5d0b4ec-ffd6-4f00-b091-e25b955d0fd2</t>
+  </si>
+  <si>
+    <t>5314d40b-d7f1-4fa9-820e-18d62d208aa9</t>
   </si>
 </sst>
 </file>
@@ -544,7 +667,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr codeName=""/>
-  <dimension ref="A1:R92"/>
+  <dimension ref="A1:R108"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1498,15 +1621,59 @@
         <v>24</v>
       </c>
     </row>
+    <row r="25">
+      <c r="A25" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="B25" s="0">
+        <v>75</v>
+      </c>
+      <c r="C25" s="0">
+        <v>90</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="F25" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G25" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="H25" s="0">
+        <v>45</v>
+      </c>
+      <c r="I25" s="0">
+        <v>35</v>
+      </c>
+      <c r="J25" s="0">
+        <v>2</v>
+      </c>
+      <c r="K25" s="0">
+        <v>90</v>
+      </c>
+      <c r="L25" s="0">
+        <v>20</v>
+      </c>
+      <c r="M25" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="N25" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
     <row r="26">
       <c r="A26" s="0" t="s">
         <v>72</v>
       </c>
       <c r="B26" s="0">
-        <v>36</v>
+        <v>75</v>
       </c>
       <c r="C26" s="0">
-        <v>36</v>
+        <v>90</v>
       </c>
       <c r="D26" s="0" t="s">
         <v>73</v>
@@ -1515,36 +1682,24 @@
         <v>74</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="G26" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="H26" s="0">
-        <v>12</v>
-      </c>
-      <c r="I26" s="0">
-        <v>10</v>
-      </c>
-      <c r="J26" s="0">
-        <v>1</v>
-      </c>
-      <c r="K26" s="0">
-        <v>12</v>
-      </c>
-      <c r="L26" s="0">
-        <v>2</v>
-      </c>
-      <c r="M26" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="O26" s="0">
         <v>75</v>
       </c>
-      <c r="N26" s="0" t="s">
-        <v>24</v>
+      <c r="P26" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q26" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="R26" s="0" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="B27" s="0">
         <v>36</v>
@@ -1553,10 +1708,10 @@
         <v>36</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="F27" s="0" t="s">
         <v>21</v>
@@ -1571,16 +1726,16 @@
         <v>10</v>
       </c>
       <c r="J27" s="0">
+        <v>1</v>
+      </c>
+      <c r="K27" s="0">
+        <v>12</v>
+      </c>
+      <c r="L27" s="0">
         <v>2</v>
       </c>
-      <c r="K27" s="0">
-        <v>24</v>
-      </c>
-      <c r="L27" s="0">
-        <v>4</v>
-      </c>
       <c r="M27" s="0" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="N27" s="0" t="s">
         <v>24</v>
@@ -1588,7 +1743,7 @@
     </row>
     <row r="28">
       <c r="A28" s="0" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="B28" s="0">
         <v>36</v>
@@ -1597,34 +1752,34 @@
         <v>36</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="F28" s="0" t="s">
         <v>21</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>77</v>
+        <v>50</v>
       </c>
       <c r="H28" s="0">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="I28" s="0">
-        <v>1.5</v>
+        <v>10</v>
       </c>
       <c r="J28" s="0">
         <v>2</v>
       </c>
       <c r="K28" s="0">
+        <v>24</v>
+      </c>
+      <c r="L28" s="0">
         <v>4</v>
       </c>
-      <c r="L28" s="0">
-        <v>1</v>
-      </c>
       <c r="M28" s="0" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="N28" s="0" t="s">
         <v>24</v>
@@ -1632,7 +1787,7 @@
     </row>
     <row r="29">
       <c r="A29" s="0" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="B29" s="0">
         <v>36</v>
@@ -1641,30 +1796,42 @@
         <v>36</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="O29" s="0">
-        <v>5</v>
-      </c>
-      <c r="P29" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="Q29" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="R29" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G29" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="H29" s="0">
+        <v>2</v>
+      </c>
+      <c r="I29" s="0">
+        <v>1.5</v>
+      </c>
+      <c r="J29" s="0">
+        <v>2</v>
+      </c>
+      <c r="K29" s="0">
+        <v>4</v>
+      </c>
+      <c r="L29" s="0">
+        <v>1</v>
+      </c>
+      <c r="M29" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="N29" s="0" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="B30" s="0">
         <v>36</v>
@@ -1673,22 +1840,22 @@
         <v>36</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="F30" s="0" t="s">
         <v>30</v>
       </c>
       <c r="O30" s="0">
-        <v>6.7</v>
+        <v>5</v>
       </c>
       <c r="P30" s="0" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="Q30" s="0" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="R30" s="0" t="s">
         <v>24</v>
@@ -1696,7 +1863,7 @@
     </row>
     <row r="31">
       <c r="A31" s="0" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="B31" s="0">
         <v>36</v>
@@ -1705,446 +1872,563 @@
         <v>36</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="F31" s="0" t="s">
         <v>30</v>
       </c>
       <c r="O31" s="0">
+        <v>6.7</v>
+      </c>
+      <c r="P31" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q31" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="R31" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="B32" s="0">
+        <v>36</v>
+      </c>
+      <c r="C32" s="0">
+        <v>36</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="E32" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="F32" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="O32" s="0">
         <v>24.3</v>
       </c>
-      <c r="P31" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="Q31" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="R31" s="0" t="s">
+      <c r="P32" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q32" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="R32" s="0" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="59">
-      <c r="A59" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="B59" s="0">
+    <row r="36">
+      <c r="A36" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="B36" s="0">
+        <v>27</v>
+      </c>
+      <c r="C36" s="0">
+        <v>25</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="E36" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="F36" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G36" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="H36" s="0">
+        <v>18</v>
+      </c>
+      <c r="I36" s="0">
+        <v>15</v>
+      </c>
+      <c r="J36" s="0">
+        <v>1</v>
+      </c>
+      <c r="K36" s="0">
+        <v>18</v>
+      </c>
+      <c r="L36" s="0">
+        <v>3</v>
+      </c>
+      <c r="M36" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="N36" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="B37" s="0">
+        <v>27</v>
+      </c>
+      <c r="C37" s="0">
+        <v>25</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="E37" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="F37" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G37" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="H37" s="0">
+        <v>7</v>
+      </c>
+      <c r="I37" s="0">
+        <v>5</v>
+      </c>
+      <c r="J37" s="0">
+        <v>1</v>
+      </c>
+      <c r="K37" s="0">
+        <v>7</v>
+      </c>
+      <c r="L37" s="0">
+        <v>2</v>
+      </c>
+      <c r="M37" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="N37" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="B38" s="0">
+        <v>27</v>
+      </c>
+      <c r="C38" s="0">
+        <v>25</v>
+      </c>
+      <c r="D38" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="E38" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="F38" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="O38" s="0">
+        <v>27</v>
+      </c>
+      <c r="P38" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q38" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="R38" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="B41" s="0">
+        <v>10</v>
+      </c>
+      <c r="C41" s="0">
         <v>20</v>
       </c>
-      <c r="C59" s="0">
-        <v>25</v>
-      </c>
-      <c r="D59" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="E59" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="F59" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="G59" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="H59" s="0">
-        <v>25</v>
-      </c>
-      <c r="I59" s="0">
+      <c r="D41" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="E41" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="F41" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G41" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H41" s="0">
         <v>20</v>
       </c>
-      <c r="J59" s="0">
-        <v>1</v>
-      </c>
-      <c r="K59" s="0">
-        <v>25</v>
-      </c>
-      <c r="L59" s="0">
-        <v>5</v>
-      </c>
-      <c r="M59" s="0" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="B60" s="0">
+      <c r="I41" s="0">
+        <v>18</v>
+      </c>
+      <c r="J41" s="0">
+        <v>1</v>
+      </c>
+      <c r="K41" s="0">
         <v>20</v>
       </c>
-      <c r="C60" s="0">
-        <v>25</v>
-      </c>
-      <c r="D60" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="E60" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="F60" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="O60" s="0">
+      <c r="L41" s="0">
+        <v>2</v>
+      </c>
+      <c r="M41" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="N41" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="B42" s="0">
+        <v>10</v>
+      </c>
+      <c r="C42" s="0">
         <v>20</v>
       </c>
-      <c r="P60" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="Q60" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="R60" s="0" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="B61" s="0">
-        <v>17.46</v>
-      </c>
-      <c r="C61" s="0">
-        <v>47</v>
-      </c>
-      <c r="D61" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="E61" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="F61" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="G61" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="H61" s="0">
-        <v>7</v>
-      </c>
-      <c r="I61" s="0">
-        <v>5</v>
-      </c>
-      <c r="J61" s="0">
-        <v>1</v>
-      </c>
-      <c r="K61" s="0">
-        <v>7</v>
-      </c>
-      <c r="L61" s="0">
+      <c r="D42" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="E42" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="F42" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="O42" s="0">
+        <v>10</v>
+      </c>
+      <c r="P42" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q42" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="R42" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="B46" s="0">
+        <v>10</v>
+      </c>
+      <c r="C46" s="0">
+        <v>12</v>
+      </c>
+      <c r="D46" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="E46" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="F46" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G46" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="H46" s="0">
+        <v>12</v>
+      </c>
+      <c r="I46" s="0">
+        <v>10</v>
+      </c>
+      <c r="J46" s="0">
+        <v>1</v>
+      </c>
+      <c r="K46" s="0">
+        <v>12</v>
+      </c>
+      <c r="L46" s="0">
         <v>2</v>
       </c>
-      <c r="M61" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="N61" s="0" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="B62" s="0">
-        <v>17.46</v>
-      </c>
-      <c r="C62" s="0">
-        <v>47</v>
-      </c>
-      <c r="D62" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="E62" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="F62" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="G62" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="H62" s="0">
+      <c r="M46" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="N46" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="B47" s="0">
         <v>10</v>
       </c>
-      <c r="I62" s="0">
-        <v>8</v>
-      </c>
-      <c r="J62" s="0">
-        <v>1</v>
-      </c>
-      <c r="K62" s="0">
+      <c r="C47" s="0">
+        <v>12</v>
+      </c>
+      <c r="D47" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="E47" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="F47" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="O47" s="0">
         <v>10</v>
       </c>
-      <c r="L62" s="0">
-        <v>2</v>
-      </c>
-      <c r="M62" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="N62" s="0" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="B63" s="0">
-        <v>17.46</v>
-      </c>
-      <c r="C63" s="0">
-        <v>47</v>
-      </c>
-      <c r="D63" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="E63" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="F63" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="G63" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="H63" s="0">
-        <v>30</v>
-      </c>
-      <c r="I63" s="0">
-        <v>15</v>
-      </c>
-      <c r="J63" s="0">
-        <v>1</v>
-      </c>
-      <c r="K63" s="0">
-        <v>30</v>
-      </c>
-      <c r="L63" s="0">
-        <v>15</v>
-      </c>
-      <c r="M63" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="N63" s="0" t="s">
-        <v>24</v>
+      <c r="P47" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q47" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="R47" s="0" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="0" t="s">
-        <v>90</v>
+        <v>109</v>
       </c>
       <c r="B64" s="0">
-        <v>17.46</v>
+        <v>20</v>
       </c>
       <c r="C64" s="0">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="D64" s="0" t="s">
-        <v>91</v>
+        <v>110</v>
       </c>
       <c r="E64" s="0" t="s">
-        <v>92</v>
+        <v>111</v>
       </c>
       <c r="F64" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="O64" s="0">
-        <v>17.46</v>
-      </c>
-      <c r="P64" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="Q64" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="R64" s="0" t="s">
-        <v>24</v>
+        <v>21</v>
+      </c>
+      <c r="G64" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="H64" s="0">
+        <v>25</v>
+      </c>
+      <c r="I64" s="0">
+        <v>20</v>
+      </c>
+      <c r="J64" s="0">
+        <v>1</v>
+      </c>
+      <c r="K64" s="0">
+        <v>25</v>
+      </c>
+      <c r="L64" s="0">
+        <v>5</v>
+      </c>
+      <c r="M64" s="0" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="0" t="s">
-        <v>97</v>
+        <v>109</v>
       </c>
       <c r="B65" s="0">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C65" s="0">
-        <v>3.5</v>
+        <v>25</v>
       </c>
       <c r="D65" s="0" t="s">
-        <v>98</v>
+        <v>110</v>
       </c>
       <c r="E65" s="0" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="F65" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="G65" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="H65" s="0">
-        <v>3.5</v>
-      </c>
-      <c r="I65" s="0">
-        <v>2</v>
-      </c>
-      <c r="J65" s="0">
-        <v>1</v>
-      </c>
-      <c r="K65" s="0">
-        <v>3.5</v>
-      </c>
-      <c r="L65" s="0">
-        <v>1.5</v>
-      </c>
-      <c r="M65" s="0" t="s">
-        <v>98</v>
+        <v>30</v>
+      </c>
+      <c r="O65" s="0">
+        <v>20</v>
+      </c>
+      <c r="P65" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q65" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="R65" s="0" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="0" t="s">
-        <v>100</v>
+        <v>115</v>
       </c>
       <c r="B66" s="0">
-        <v>15</v>
+        <v>17.46</v>
       </c>
       <c r="C66" s="0">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="D66" s="0" t="s">
-        <v>101</v>
+        <v>116</v>
       </c>
       <c r="E66" s="0" t="s">
-        <v>102</v>
+        <v>117</v>
       </c>
       <c r="F66" s="0" t="s">
         <v>21</v>
       </c>
       <c r="G66" s="0" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="H66" s="0">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="I66" s="0">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="J66" s="0">
         <v>1</v>
       </c>
       <c r="K66" s="0">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="L66" s="0">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="M66" s="0" t="s">
-        <v>101</v>
+        <v>118</v>
+      </c>
+      <c r="N66" s="0" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="0" t="s">
-        <v>100</v>
+        <v>115</v>
       </c>
       <c r="B67" s="0">
-        <v>15</v>
+        <v>17.46</v>
       </c>
       <c r="C67" s="0">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="D67" s="0" t="s">
-        <v>101</v>
+        <v>116</v>
       </c>
       <c r="E67" s="0" t="s">
-        <v>102</v>
+        <v>117</v>
       </c>
       <c r="F67" s="0" t="s">
         <v>21</v>
       </c>
       <c r="G67" s="0" t="s">
-        <v>77</v>
+        <v>119</v>
       </c>
       <c r="H67" s="0">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="I67" s="0">
-        <v>1.5</v>
+        <v>8</v>
       </c>
       <c r="J67" s="0">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K67" s="0">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="L67" s="0">
         <v>2</v>
       </c>
       <c r="M67" s="0" t="s">
-        <v>101</v>
+        <v>118</v>
+      </c>
+      <c r="N67" s="0" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="0" t="s">
-        <v>100</v>
+        <v>115</v>
       </c>
       <c r="B68" s="0">
+        <v>17.46</v>
+      </c>
+      <c r="C68" s="0">
+        <v>47</v>
+      </c>
+      <c r="D68" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="E68" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="F68" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G68" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="H68" s="0">
+        <v>30</v>
+      </c>
+      <c r="I68" s="0">
         <v>15</v>
       </c>
-      <c r="C68" s="0">
-        <v>33</v>
-      </c>
-      <c r="D68" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="E68" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="F68" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="O68" s="0">
-        <v>5</v>
-      </c>
-      <c r="P68" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="Q68" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="R68" s="0" t="s">
+      <c r="J68" s="0">
+        <v>1</v>
+      </c>
+      <c r="K68" s="0">
+        <v>30</v>
+      </c>
+      <c r="L68" s="0">
+        <v>15</v>
+      </c>
+      <c r="M68" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="N68" s="0" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="0" t="s">
-        <v>100</v>
+        <v>115</v>
       </c>
       <c r="B69" s="0">
-        <v>15</v>
+        <v>17.46</v>
       </c>
       <c r="C69" s="0">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="D69" s="0" t="s">
-        <v>101</v>
+        <v>116</v>
       </c>
       <c r="E69" s="0" t="s">
-        <v>102</v>
+        <v>117</v>
       </c>
       <c r="F69" s="0" t="s">
         <v>30</v>
       </c>
       <c r="O69" s="0">
-        <v>10</v>
+        <v>17.46</v>
       </c>
       <c r="P69" s="0" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="Q69" s="0" t="s">
-        <v>107</v>
+        <v>120</v>
       </c>
       <c r="R69" s="0" t="s">
         <v>24</v>
@@ -2152,130 +2436,142 @@
     </row>
     <row r="70">
       <c r="A70" s="0" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="B70" s="0">
-        <v>400</v>
+        <v>0</v>
       </c>
       <c r="C70" s="0">
-        <v>500</v>
+        <v>3.5</v>
       </c>
       <c r="D70" s="0" t="s">
-        <v>109</v>
+        <v>122</v>
       </c>
       <c r="E70" s="0" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="F70" s="0" t="s">
         <v>21</v>
       </c>
       <c r="G70" s="0" t="s">
-        <v>111</v>
+        <v>58</v>
       </c>
       <c r="H70" s="0">
-        <v>500</v>
+        <v>3.5</v>
       </c>
       <c r="I70" s="0">
-        <v>250</v>
+        <v>2</v>
       </c>
       <c r="J70" s="0">
         <v>1</v>
       </c>
       <c r="K70" s="0">
-        <v>500</v>
+        <v>3.5</v>
       </c>
       <c r="L70" s="0">
-        <v>250</v>
+        <v>1.5</v>
       </c>
       <c r="M70" s="0" t="s">
-        <v>109</v>
+        <v>122</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="0" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
       <c r="B71" s="0">
-        <v>400</v>
+        <v>15</v>
       </c>
       <c r="C71" s="0">
-        <v>500</v>
+        <v>33</v>
       </c>
       <c r="D71" s="0" t="s">
-        <v>109</v>
+        <v>125</v>
       </c>
       <c r="E71" s="0" t="s">
-        <v>110</v>
+        <v>126</v>
       </c>
       <c r="F71" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="O71" s="0">
-        <v>400</v>
-      </c>
-      <c r="P71" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="Q71" s="0" t="s">
-        <v>112</v>
+        <v>21</v>
+      </c>
+      <c r="G71" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="H71" s="0">
+        <v>25</v>
+      </c>
+      <c r="I71" s="0">
+        <v>18</v>
+      </c>
+      <c r="J71" s="0">
+        <v>1</v>
+      </c>
+      <c r="K71" s="0">
+        <v>25</v>
+      </c>
+      <c r="L71" s="0">
+        <v>7</v>
+      </c>
+      <c r="M71" s="0" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="0" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="B72" s="0">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="C72" s="0">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="D72" s="0" t="s">
-        <v>114</v>
+        <v>125</v>
       </c>
       <c r="E72" s="0" t="s">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="F72" s="0" t="s">
         <v>21</v>
       </c>
       <c r="G72" s="0" t="s">
-        <v>116</v>
+        <v>83</v>
       </c>
       <c r="H72" s="0">
-        <v>4.5</v>
+        <v>2</v>
       </c>
       <c r="I72" s="0">
-        <v>2.5</v>
+        <v>1.5</v>
       </c>
       <c r="J72" s="0">
+        <v>4</v>
+      </c>
+      <c r="K72" s="0">
+        <v>8</v>
+      </c>
+      <c r="L72" s="0">
         <v>2</v>
       </c>
-      <c r="K72" s="0">
-        <v>9</v>
-      </c>
-      <c r="L72" s="0">
-        <v>4</v>
-      </c>
       <c r="M72" s="0" t="s">
-        <v>114</v>
+        <v>125</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="0" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="B73" s="0">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="C73" s="0">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="D73" s="0" t="s">
-        <v>114</v>
+        <v>125</v>
       </c>
       <c r="E73" s="0" t="s">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="F73" s="0" t="s">
         <v>30</v>
@@ -2284,684 +2580,1274 @@
         <v>5</v>
       </c>
       <c r="P73" s="0" t="s">
-        <v>114</v>
+        <v>128</v>
       </c>
       <c r="Q73" s="0" t="s">
-        <v>117</v>
+        <v>129</v>
+      </c>
+      <c r="R73" s="0" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="0" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="B74" s="0">
-        <v>100</v>
+        <v>15</v>
       </c>
       <c r="C74" s="0">
-        <v>120</v>
+        <v>33</v>
       </c>
       <c r="D74" s="0" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="E74" s="0" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="F74" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="G74" s="0" t="s">
-        <v>121</v>
-      </c>
-      <c r="H74" s="0">
-        <v>120</v>
-      </c>
-      <c r="I74" s="0">
-        <v>90</v>
-      </c>
-      <c r="J74" s="0">
-        <v>1</v>
-      </c>
-      <c r="K74" s="0">
-        <v>120</v>
-      </c>
-      <c r="L74" s="0">
-        <v>30</v>
-      </c>
-      <c r="M74" s="0" t="s">
-        <v>119</v>
+        <v>30</v>
+      </c>
+      <c r="O74" s="0">
+        <v>10</v>
+      </c>
+      <c r="P74" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q74" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="R74" s="0" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="0" t="s">
-        <v>118</v>
+        <v>132</v>
       </c>
       <c r="B75" s="0">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="C75" s="0">
-        <v>120</v>
+        <v>500</v>
       </c>
       <c r="D75" s="0" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="E75" s="0" t="s">
-        <v>120</v>
+        <v>134</v>
       </c>
       <c r="F75" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="O75" s="0">
-        <v>100</v>
-      </c>
-      <c r="P75" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="Q75" s="0" t="s">
-        <v>122</v>
+        <v>21</v>
+      </c>
+      <c r="G75" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="H75" s="0">
+        <v>500</v>
+      </c>
+      <c r="I75" s="0">
+        <v>250</v>
+      </c>
+      <c r="J75" s="0">
+        <v>1</v>
+      </c>
+      <c r="K75" s="0">
+        <v>500</v>
+      </c>
+      <c r="L75" s="0">
+        <v>250</v>
+      </c>
+      <c r="M75" s="0" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="0" t="s">
-        <v>123</v>
+        <v>132</v>
       </c>
       <c r="B76" s="0">
-        <v>30</v>
+        <v>400</v>
       </c>
       <c r="C76" s="0">
-        <v>45</v>
+        <v>500</v>
       </c>
       <c r="D76" s="0" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="E76" s="0" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="F76" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="G76" s="0" t="s">
-        <v>126</v>
-      </c>
-      <c r="H76" s="0">
-        <v>45</v>
-      </c>
-      <c r="I76" s="0">
-        <v>35</v>
-      </c>
-      <c r="J76" s="0">
-        <v>1</v>
-      </c>
-      <c r="K76" s="0">
-        <v>45</v>
-      </c>
-      <c r="L76" s="0">
-        <v>10</v>
-      </c>
-      <c r="M76" s="0" t="s">
-        <v>124</v>
+        <v>30</v>
+      </c>
+      <c r="O76" s="0">
+        <v>400</v>
+      </c>
+      <c r="P76" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="Q76" s="0" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="0" t="s">
-        <v>123</v>
+        <v>137</v>
       </c>
       <c r="B77" s="0">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="C77" s="0">
-        <v>45</v>
+        <v>9</v>
       </c>
       <c r="D77" s="0" t="s">
-        <v>124</v>
+        <v>138</v>
       </c>
       <c r="E77" s="0" t="s">
-        <v>125</v>
+        <v>139</v>
       </c>
       <c r="F77" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="O77" s="0">
-        <v>30</v>
-      </c>
-      <c r="P77" s="0" t="s">
-        <v>124</v>
-      </c>
-      <c r="Q77" s="0" t="s">
-        <v>127</v>
+        <v>21</v>
+      </c>
+      <c r="G77" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="H77" s="0">
+        <v>4.5</v>
+      </c>
+      <c r="I77" s="0">
+        <v>2.5</v>
+      </c>
+      <c r="J77" s="0">
+        <v>2</v>
+      </c>
+      <c r="K77" s="0">
+        <v>9</v>
+      </c>
+      <c r="L77" s="0">
+        <v>4</v>
+      </c>
+      <c r="M77" s="0" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="0" t="s">
-        <v>128</v>
+        <v>137</v>
       </c>
       <c r="B78" s="0">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C78" s="0">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D78" s="0" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="E78" s="0" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="F78" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="G78" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="H78" s="0">
-        <v>7</v>
-      </c>
-      <c r="I78" s="0">
+        <v>30</v>
+      </c>
+      <c r="O78" s="0">
         <v>5</v>
       </c>
-      <c r="J78" s="0">
-        <v>1</v>
-      </c>
-      <c r="K78" s="0">
-        <v>7</v>
-      </c>
-      <c r="L78" s="0">
-        <v>2</v>
-      </c>
-      <c r="M78" s="0" t="s">
-        <v>129</v>
+      <c r="P78" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q78" s="0" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="0" t="s">
-        <v>128</v>
+        <v>142</v>
       </c>
       <c r="B79" s="0">
-        <v>6</v>
+        <v>100</v>
       </c>
       <c r="C79" s="0">
-        <v>7</v>
+        <v>120</v>
       </c>
       <c r="D79" s="0" t="s">
-        <v>129</v>
+        <v>143</v>
       </c>
       <c r="E79" s="0" t="s">
-        <v>130</v>
+        <v>144</v>
       </c>
       <c r="F79" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="O79" s="0">
-        <v>6</v>
-      </c>
-      <c r="P79" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="Q79" s="0" t="s">
-        <v>131</v>
+        <v>21</v>
+      </c>
+      <c r="G79" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="H79" s="0">
+        <v>120</v>
+      </c>
+      <c r="I79" s="0">
+        <v>90</v>
+      </c>
+      <c r="J79" s="0">
+        <v>1</v>
+      </c>
+      <c r="K79" s="0">
+        <v>120</v>
+      </c>
+      <c r="L79" s="0">
+        <v>30</v>
+      </c>
+      <c r="M79" s="0" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="0" t="s">
-        <v>132</v>
+        <v>142</v>
       </c>
       <c r="B80" s="0">
-        <v>35</v>
+        <v>100</v>
       </c>
       <c r="C80" s="0">
-        <v>45</v>
+        <v>120</v>
       </c>
       <c r="D80" s="0" t="s">
-        <v>133</v>
+        <v>143</v>
       </c>
       <c r="E80" s="0" t="s">
-        <v>134</v>
+        <v>144</v>
       </c>
       <c r="F80" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="G80" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="H80" s="0">
-        <v>15</v>
-      </c>
-      <c r="I80" s="0">
-        <v>10</v>
-      </c>
-      <c r="J80" s="0">
-        <v>3</v>
-      </c>
-      <c r="K80" s="0">
-        <v>45</v>
-      </c>
-      <c r="L80" s="0">
-        <v>15</v>
-      </c>
-      <c r="M80" s="0" t="s">
-        <v>133</v>
+        <v>30</v>
+      </c>
+      <c r="O80" s="0">
+        <v>100</v>
+      </c>
+      <c r="P80" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q80" s="0" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="0" t="s">
-        <v>132</v>
+        <v>147</v>
       </c>
       <c r="B81" s="0">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C81" s="0">
         <v>45</v>
       </c>
       <c r="D81" s="0" t="s">
-        <v>133</v>
+        <v>148</v>
       </c>
       <c r="E81" s="0" t="s">
-        <v>134</v>
+        <v>149</v>
       </c>
       <c r="F81" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="O81" s="0">
+        <v>21</v>
+      </c>
+      <c r="G81" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="H81" s="0">
+        <v>45</v>
+      </c>
+      <c r="I81" s="0">
         <v>35</v>
       </c>
-      <c r="P81" s="0" t="s">
-        <v>135</v>
-      </c>
-      <c r="Q81" s="0" t="s">
-        <v>136</v>
-      </c>
-      <c r="R81" s="0" t="s">
-        <v>60</v>
+      <c r="J81" s="0">
+        <v>1</v>
+      </c>
+      <c r="K81" s="0">
+        <v>45</v>
+      </c>
+      <c r="L81" s="0">
+        <v>10</v>
+      </c>
+      <c r="M81" s="0" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="0" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
       <c r="B82" s="0">
-        <v>14.56</v>
+        <v>30</v>
       </c>
       <c r="C82" s="0">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D82" s="0" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="E82" s="0" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="F82" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="G82" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="H82" s="0">
-        <v>25</v>
-      </c>
-      <c r="I82" s="0">
-        <v>20</v>
-      </c>
-      <c r="J82" s="0">
-        <v>1</v>
-      </c>
-      <c r="K82" s="0">
-        <v>25</v>
-      </c>
-      <c r="L82" s="0">
-        <v>5</v>
-      </c>
-      <c r="M82" s="0" t="s">
-        <v>138</v>
+        <v>30</v>
+      </c>
+      <c r="O82" s="0">
+        <v>30</v>
+      </c>
+      <c r="P82" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="Q82" s="0" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="0" t="s">
-        <v>137</v>
+        <v>151</v>
       </c>
       <c r="B83" s="0">
-        <v>14.56</v>
+        <v>6</v>
       </c>
       <c r="C83" s="0">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="D83" s="0" t="s">
-        <v>138</v>
+        <v>152</v>
       </c>
       <c r="E83" s="0" t="s">
-        <v>139</v>
+        <v>153</v>
       </c>
       <c r="F83" s="0" t="s">
         <v>21</v>
       </c>
       <c r="G83" s="0" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="H83" s="0">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="I83" s="0">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="J83" s="0">
         <v>1</v>
       </c>
       <c r="K83" s="0">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="L83" s="0">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="M83" s="0" t="s">
-        <v>138</v>
+        <v>152</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="0" t="s">
-        <v>137</v>
+        <v>151</v>
       </c>
       <c r="B84" s="0">
-        <v>14.56</v>
+        <v>6</v>
       </c>
       <c r="C84" s="0">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="D84" s="0" t="s">
-        <v>138</v>
+        <v>152</v>
       </c>
       <c r="E84" s="0" t="s">
-        <v>139</v>
+        <v>153</v>
       </c>
       <c r="F84" s="0" t="s">
         <v>30</v>
       </c>
       <c r="O84" s="0">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="P84" s="0" t="s">
-        <v>138</v>
+        <v>152</v>
       </c>
       <c r="Q84" s="0" t="s">
-        <v>140</v>
+        <v>154</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="0" t="s">
-        <v>137</v>
+        <v>155</v>
       </c>
       <c r="B85" s="0">
-        <v>14.56</v>
+        <v>35</v>
       </c>
       <c r="C85" s="0">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D85" s="0" t="s">
-        <v>138</v>
+        <v>156</v>
       </c>
       <c r="E85" s="0" t="s">
-        <v>139</v>
+        <v>157</v>
       </c>
       <c r="F85" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="O85" s="0">
-        <v>4.56</v>
-      </c>
-      <c r="P85" s="0" t="s">
-        <v>141</v>
-      </c>
-      <c r="Q85" s="0" t="s">
-        <v>142</v>
-      </c>
-      <c r="R85" s="0" t="s">
-        <v>42</v>
+        <v>21</v>
+      </c>
+      <c r="G85" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="H85" s="0">
+        <v>15</v>
+      </c>
+      <c r="I85" s="0">
+        <v>10</v>
+      </c>
+      <c r="J85" s="0">
+        <v>3</v>
+      </c>
+      <c r="K85" s="0">
+        <v>45</v>
+      </c>
+      <c r="L85" s="0">
+        <v>15</v>
+      </c>
+      <c r="M85" s="0" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="0" t="s">
-        <v>143</v>
+        <v>155</v>
       </c>
       <c r="B86" s="0">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="C86" s="0">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="D86" s="0" t="s">
-        <v>144</v>
+        <v>156</v>
       </c>
       <c r="E86" s="0" t="s">
-        <v>145</v>
+        <v>157</v>
       </c>
       <c r="F86" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="G86" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="H86" s="0">
-        <v>25</v>
-      </c>
-      <c r="I86" s="0">
-        <v>18</v>
-      </c>
-      <c r="J86" s="0">
-        <v>1</v>
-      </c>
-      <c r="K86" s="0">
-        <v>25</v>
-      </c>
-      <c r="L86" s="0">
-        <v>7</v>
-      </c>
-      <c r="M86" s="0" t="s">
-        <v>144</v>
+        <v>30</v>
+      </c>
+      <c r="O86" s="0">
+        <v>35</v>
+      </c>
+      <c r="P86" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q86" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="R86" s="0" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="0" t="s">
-        <v>143</v>
+        <v>160</v>
       </c>
       <c r="B87" s="0">
+        <v>14.56</v>
+      </c>
+      <c r="C87" s="0">
+        <v>50</v>
+      </c>
+      <c r="D87" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="E87" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="F87" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G87" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="H87" s="0">
         <v>25</v>
       </c>
-      <c r="C87" s="0">
+      <c r="I87" s="0">
+        <v>20</v>
+      </c>
+      <c r="J87" s="0">
+        <v>1</v>
+      </c>
+      <c r="K87" s="0">
         <v>25</v>
       </c>
-      <c r="D87" s="0" t="s">
-        <v>144</v>
-      </c>
-      <c r="E87" s="0" t="s">
-        <v>145</v>
-      </c>
-      <c r="F87" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="O87" s="0">
-        <v>25</v>
-      </c>
-      <c r="P87" s="0" t="s">
-        <v>146</v>
-      </c>
-      <c r="Q87" s="0" t="s">
-        <v>147</v>
-      </c>
-      <c r="R87" s="0" t="s">
-        <v>148</v>
+      <c r="L87" s="0">
+        <v>5</v>
+      </c>
+      <c r="M87" s="0" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="0" t="s">
-        <v>149</v>
+        <v>160</v>
       </c>
       <c r="B88" s="0">
-        <v>500</v>
+        <v>14.56</v>
       </c>
       <c r="C88" s="0">
-        <v>500</v>
+        <v>50</v>
       </c>
       <c r="D88" s="0" t="s">
-        <v>150</v>
+        <v>161</v>
       </c>
       <c r="E88" s="0" t="s">
-        <v>151</v>
+        <v>162</v>
       </c>
       <c r="F88" s="0" t="s">
         <v>21</v>
       </c>
       <c r="G88" s="0" t="s">
-        <v>111</v>
+        <v>127</v>
       </c>
       <c r="H88" s="0">
-        <v>500</v>
+        <v>25</v>
       </c>
       <c r="I88" s="0">
-        <v>250</v>
+        <v>18</v>
       </c>
       <c r="J88" s="0">
         <v>1</v>
       </c>
       <c r="K88" s="0">
-        <v>500</v>
+        <v>25</v>
       </c>
       <c r="L88" s="0">
-        <v>250</v>
+        <v>7</v>
       </c>
       <c r="M88" s="0" t="s">
-        <v>150</v>
+        <v>161</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="0" t="s">
-        <v>149</v>
+        <v>160</v>
       </c>
       <c r="B89" s="0">
-        <v>500</v>
+        <v>14.56</v>
       </c>
       <c r="C89" s="0">
-        <v>500</v>
+        <v>50</v>
       </c>
       <c r="D89" s="0" t="s">
-        <v>150</v>
+        <v>161</v>
       </c>
       <c r="E89" s="0" t="s">
-        <v>151</v>
+        <v>162</v>
       </c>
       <c r="F89" s="0" t="s">
         <v>30</v>
       </c>
       <c r="O89" s="0">
-        <v>400</v>
+        <v>10</v>
       </c>
       <c r="P89" s="0" t="s">
-        <v>150</v>
+        <v>161</v>
       </c>
       <c r="Q89" s="0" t="s">
-        <v>152</v>
+        <v>163</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="0" t="s">
-        <v>149</v>
+        <v>160</v>
       </c>
       <c r="B90" s="0">
-        <v>500</v>
+        <v>14.56</v>
       </c>
       <c r="C90" s="0">
-        <v>500</v>
+        <v>50</v>
       </c>
       <c r="D90" s="0" t="s">
-        <v>150</v>
+        <v>161</v>
       </c>
       <c r="E90" s="0" t="s">
-        <v>151</v>
+        <v>162</v>
       </c>
       <c r="F90" s="0" t="s">
         <v>30</v>
       </c>
       <c r="O90" s="0">
-        <v>100</v>
+        <v>4.56</v>
       </c>
       <c r="P90" s="0" t="s">
-        <v>153</v>
+        <v>164</v>
       </c>
       <c r="Q90" s="0" t="s">
-        <v>154</v>
+        <v>165</v>
       </c>
       <c r="R90" s="0" t="s">
-        <v>148</v>
+        <v>42</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="0" t="s">
-        <v>155</v>
+        <v>166</v>
       </c>
       <c r="B91" s="0">
-        <v>13.5</v>
+        <v>25</v>
       </c>
       <c r="C91" s="0">
-        <v>13.5</v>
+        <v>12</v>
       </c>
       <c r="D91" s="0" t="s">
-        <v>156</v>
+        <v>167</v>
       </c>
       <c r="E91" s="0" t="s">
-        <v>157</v>
+        <v>168</v>
       </c>
       <c r="F91" s="0" t="s">
         <v>21</v>
       </c>
       <c r="G91" s="0" t="s">
-        <v>116</v>
+        <v>127</v>
       </c>
       <c r="H91" s="0">
-        <v>4.5</v>
+        <v>25</v>
       </c>
       <c r="I91" s="0">
-        <v>2.5</v>
+        <v>18</v>
       </c>
       <c r="J91" s="0">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K91" s="0">
-        <v>13.5</v>
+        <v>25</v>
       </c>
       <c r="L91" s="0">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M91" s="0" t="s">
-        <v>156</v>
+        <v>167</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="0" t="s">
-        <v>155</v>
+        <v>166</v>
       </c>
       <c r="B92" s="0">
+        <v>25</v>
+      </c>
+      <c r="C92" s="0">
+        <v>12</v>
+      </c>
+      <c r="D92" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="E92" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="F92" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G92" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="H92" s="0">
+        <v>12</v>
+      </c>
+      <c r="I92" s="0">
+        <v>10</v>
+      </c>
+      <c r="J92" s="0">
+        <v>1</v>
+      </c>
+      <c r="K92" s="0">
+        <v>12</v>
+      </c>
+      <c r="L92" s="0">
+        <v>2</v>
+      </c>
+      <c r="M92" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="N92" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="B93" s="0">
+        <v>25</v>
+      </c>
+      <c r="C93" s="0">
+        <v>12</v>
+      </c>
+      <c r="D93" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="E93" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="F93" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="O93" s="0">
+        <v>25</v>
+      </c>
+      <c r="P93" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="Q93" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="R93" s="0" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="B94" s="0">
+        <v>500</v>
+      </c>
+      <c r="C94" s="0">
+        <v>500</v>
+      </c>
+      <c r="D94" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="E94" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="F94" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G94" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="H94" s="0">
+        <v>500</v>
+      </c>
+      <c r="I94" s="0">
+        <v>250</v>
+      </c>
+      <c r="J94" s="0">
+        <v>1</v>
+      </c>
+      <c r="K94" s="0">
+        <v>500</v>
+      </c>
+      <c r="L94" s="0">
+        <v>250</v>
+      </c>
+      <c r="M94" s="0" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="B95" s="0">
+        <v>500</v>
+      </c>
+      <c r="C95" s="0">
+        <v>500</v>
+      </c>
+      <c r="D95" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="E95" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="F95" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="O95" s="0">
+        <v>400</v>
+      </c>
+      <c r="P95" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="Q95" s="0" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="B96" s="0">
+        <v>500</v>
+      </c>
+      <c r="C96" s="0">
+        <v>500</v>
+      </c>
+      <c r="D96" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="E96" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="F96" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="O96" s="0">
+        <v>100</v>
+      </c>
+      <c r="P96" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="Q96" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="R96" s="0" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="B97" s="0">
         <v>13.5</v>
       </c>
-      <c r="C92" s="0">
+      <c r="C97" s="0">
         <v>13.5</v>
       </c>
-      <c r="D92" s="0" t="s">
-        <v>156</v>
-      </c>
-      <c r="E92" s="0" t="s">
-        <v>157</v>
-      </c>
-      <c r="F92" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="O92" s="0">
+      <c r="D97" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="E97" s="0" t="s">
+        <v>182</v>
+      </c>
+      <c r="F97" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G97" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="H97" s="0">
+        <v>4.5</v>
+      </c>
+      <c r="I97" s="0">
+        <v>2.5</v>
+      </c>
+      <c r="J97" s="0">
+        <v>3</v>
+      </c>
+      <c r="K97" s="0">
         <v>13.5</v>
       </c>
-      <c r="P92" s="0" t="s">
-        <v>158</v>
-      </c>
-      <c r="Q92" s="0" t="s">
-        <v>159</v>
-      </c>
-      <c r="R92" s="0" t="s">
-        <v>148</v>
+      <c r="L97" s="0">
+        <v>6</v>
+      </c>
+      <c r="M97" s="0" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="B98" s="0">
+        <v>13.5</v>
+      </c>
+      <c r="C98" s="0">
+        <v>13.5</v>
+      </c>
+      <c r="D98" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="E98" s="0" t="s">
+        <v>182</v>
+      </c>
+      <c r="F98" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="O98" s="0">
+        <v>13.5</v>
+      </c>
+      <c r="P98" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="Q98" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="R98" s="0" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="B99" s="0">
+        <v>40</v>
+      </c>
+      <c r="C99" s="0">
+        <v>40</v>
+      </c>
+      <c r="D99" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="E99" s="0" t="s">
+        <v>187</v>
+      </c>
+      <c r="F99" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G99" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="H99" s="0">
+        <v>30</v>
+      </c>
+      <c r="I99" s="0">
+        <v>15</v>
+      </c>
+      <c r="J99" s="0">
+        <v>1</v>
+      </c>
+      <c r="K99" s="0">
+        <v>30</v>
+      </c>
+      <c r="L99" s="0">
+        <v>15</v>
+      </c>
+      <c r="M99" s="0" t="s">
+        <v>188</v>
+      </c>
+      <c r="N99" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="B100" s="0">
+        <v>40</v>
+      </c>
+      <c r="C100" s="0">
+        <v>40</v>
+      </c>
+      <c r="D100" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="E100" s="0" t="s">
+        <v>187</v>
+      </c>
+      <c r="F100" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G100" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="H100" s="0">
+        <v>10</v>
+      </c>
+      <c r="I100" s="0">
+        <v>8</v>
+      </c>
+      <c r="J100" s="0">
+        <v>1</v>
+      </c>
+      <c r="K100" s="0">
+        <v>10</v>
+      </c>
+      <c r="L100" s="0">
+        <v>2</v>
+      </c>
+      <c r="M100" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="N100" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="B101" s="0">
+        <v>40</v>
+      </c>
+      <c r="C101" s="0">
+        <v>40</v>
+      </c>
+      <c r="D101" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="E101" s="0" t="s">
+        <v>187</v>
+      </c>
+      <c r="F101" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G101" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="H101" s="0">
+        <v>2</v>
+      </c>
+      <c r="I101" s="0">
+        <v>1.5</v>
+      </c>
+      <c r="J101" s="0">
+        <v>1</v>
+      </c>
+      <c r="K101" s="0">
+        <v>2</v>
+      </c>
+      <c r="L101" s="0">
+        <v>0.5</v>
+      </c>
+      <c r="M101" s="0" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="B102" s="0">
+        <v>40</v>
+      </c>
+      <c r="C102" s="0">
+        <v>40</v>
+      </c>
+      <c r="D102" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="E102" s="0" t="s">
+        <v>187</v>
+      </c>
+      <c r="F102" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="O102" s="0">
+        <v>2</v>
+      </c>
+      <c r="P102" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q102" s="0" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="B103" s="0">
+        <v>40</v>
+      </c>
+      <c r="C103" s="0">
+        <v>40</v>
+      </c>
+      <c r="D103" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="E103" s="0" t="s">
+        <v>187</v>
+      </c>
+      <c r="F103" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="O103" s="0">
+        <v>38</v>
+      </c>
+      <c r="P103" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="Q103" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="R103" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="B104" s="0">
+        <v>70</v>
+      </c>
+      <c r="C104" s="0">
+        <v>115</v>
+      </c>
+      <c r="D104" s="0" t="s">
+        <v>194</v>
+      </c>
+      <c r="E104" s="0" t="s">
+        <v>195</v>
+      </c>
+      <c r="F104" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G104" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="H104" s="0">
+        <v>80</v>
+      </c>
+      <c r="I104" s="0">
+        <v>60</v>
+      </c>
+      <c r="J104" s="0">
+        <v>1</v>
+      </c>
+      <c r="K104" s="0">
+        <v>80</v>
+      </c>
+      <c r="L104" s="0">
+        <v>20</v>
+      </c>
+      <c r="M104" s="0" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="B105" s="0">
+        <v>70</v>
+      </c>
+      <c r="C105" s="0">
+        <v>115</v>
+      </c>
+      <c r="D105" s="0" t="s">
+        <v>194</v>
+      </c>
+      <c r="E105" s="0" t="s">
+        <v>195</v>
+      </c>
+      <c r="F105" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G105" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="H105" s="0">
+        <v>35</v>
+      </c>
+      <c r="I105" s="0">
+        <v>30</v>
+      </c>
+      <c r="J105" s="0">
+        <v>1</v>
+      </c>
+      <c r="K105" s="0">
+        <v>35</v>
+      </c>
+      <c r="L105" s="0">
+        <v>5</v>
+      </c>
+      <c r="M105" s="0" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="B106" s="0">
+        <v>70</v>
+      </c>
+      <c r="C106" s="0">
+        <v>115</v>
+      </c>
+      <c r="D106" s="0" t="s">
+        <v>194</v>
+      </c>
+      <c r="E106" s="0" t="s">
+        <v>195</v>
+      </c>
+      <c r="F106" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="O106" s="0">
+        <v>70</v>
+      </c>
+      <c r="P106" s="0" t="s">
+        <v>194</v>
+      </c>
+      <c r="Q106" s="0" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="B107" s="0">
+        <v>120</v>
+      </c>
+      <c r="C107" s="0">
+        <v>120</v>
+      </c>
+      <c r="D107" s="0" t="s">
+        <v>198</v>
+      </c>
+      <c r="E107" s="0" t="s">
+        <v>199</v>
+      </c>
+      <c r="F107" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G107" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="H107" s="0">
+        <v>120</v>
+      </c>
+      <c r="I107" s="0">
+        <v>90</v>
+      </c>
+      <c r="J107" s="0">
+        <v>1</v>
+      </c>
+      <c r="K107" s="0">
+        <v>120</v>
+      </c>
+      <c r="L107" s="0">
+        <v>30</v>
+      </c>
+      <c r="M107" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="B108" s="0">
+        <v>120</v>
+      </c>
+      <c r="C108" s="0">
+        <v>120</v>
+      </c>
+      <c r="D108" s="0" t="s">
+        <v>198</v>
+      </c>
+      <c r="E108" s="0" t="s">
+        <v>199</v>
+      </c>
+      <c r="F108" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="O108" s="0">
+        <v>120</v>
+      </c>
+      <c r="P108" s="0" t="s">
+        <v>198</v>
+      </c>
+      <c r="Q108" s="0" t="s">
+        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>